<commit_message>
only display digits each frame if t > 1
</commit_message>
<xml_diff>
--- a/html/resources/three.xlsx
+++ b/html/resources/three.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Digit Span\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adkinsty/files/experiments/digit-span-backward/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DF0C249-B951-42F2-801C-88850AB65328}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE3BFCF-4151-BE42-838B-538CDA943F04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B186CD21-A5B9-412D-9520-9926A5EF8780}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11160" xr2:uid="{B186CD21-A5B9-412D-9520-9926A5EF8780}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,15 +391,15 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B31"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -415,7 +415,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -423,7 +423,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>

</xml_diff>